<commit_message>
Python script for project
</commit_message>
<xml_diff>
--- a/datasets/2023_NFL_receiving_stats.xlsx
+++ b/datasets/2023_NFL_receiving_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sumailsyr-my.sharepoint.com/personal/rpmichae_syr_edu/Documents/SAL 603/repositories/FinalProject/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{7DE4A10D-F67E-694C-9507-B32D4914B84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DE50466-9F5B-E94C-BD7E-AB8FA69B85C7}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{7DE4A10D-F67E-694C-9507-B32D4914B84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5A8EBFA-C566-9347-8B31-CBA04E5156BE}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{477392A5-DB56-364F-9AC9-D005DAF9394F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1029">
   <si>
     <t>Rk</t>
   </si>
@@ -3120,6 +3120,9 @@
   </si>
   <si>
     <t>Pos</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -3481,7 +3484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54EE6A9-3B61-7244-9FB5-E0E3C4C53B20}">
   <dimension ref="A1:U483"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3838,8 +3843,8 @@
       <c r="I6">
         <v>35</v>
       </c>
-      <c r="J6" s="2">
-        <v>0.77800000000000002</v>
+      <c r="J6" s="2" t="s">
+        <v>1028</v>
       </c>
       <c r="K6">
         <v>381</v>

</xml_diff>